<commit_message>
[update images and ipynotebook]
</commit_message>
<xml_diff>
--- a/MA_Stock_Table.xlsx
+++ b/MA_Stock_Table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Python-DataAnalysis-FInancialEvent-Lejie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F6D30F1A-4FD8-4B56-A906-7098C5B1130C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD25FA7E-6CE1-4260-9B5D-C1BA5A4C0E4C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{18CE2C7B-F3D7-445C-8E2F-807BAFD5D61E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{18CE2C7B-F3D7-445C-8E2F-807BAFD5D61E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2744" uniqueCount="1078">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3072" uniqueCount="1080">
   <si>
     <t>Changzhou (city)</t>
   </si>
@@ -3268,6 +3268,14 @@
   </si>
   <si>
     <t>EventID</t>
+  </si>
+  <si>
+    <t>China</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Country</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3636,18 +3644,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D710CB-B9E7-4B16-A4AB-265A902EB329}">
-  <dimension ref="A1:CY328"/>
+  <dimension ref="A1:CZ328"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="CL1" workbookViewId="0">
+      <selection activeCell="DA8" sqref="DA8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="8" max="49" width="11.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="13.125" customWidth="1"/>
+    <col min="104" max="104" width="10.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1077</v>
       </c>
@@ -3951,8 +3961,11 @@
       <c r="CY1" t="s">
         <v>1059</v>
       </c>
+      <c r="CZ1" t="s">
+        <v>1079</v>
+      </c>
     </row>
-    <row r="2" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1058</v>
       </c>
@@ -4253,8 +4266,11 @@
       <c r="CY2">
         <v>0</v>
       </c>
+      <c r="CZ2" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="3" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1056</v>
       </c>
@@ -4555,8 +4571,11 @@
       <c r="CY3" t="s">
         <v>51</v>
       </c>
+      <c r="CZ3" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="4" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1053</v>
       </c>
@@ -4857,8 +4876,11 @@
       <c r="CY4" t="s">
         <v>22</v>
       </c>
+      <c r="CZ4" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="5" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1050</v>
       </c>
@@ -5159,8 +5181,11 @@
       <c r="CY5" t="s">
         <v>654</v>
       </c>
+      <c r="CZ5" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="6" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>1048</v>
       </c>
@@ -5461,8 +5486,11 @@
       <c r="CY6">
         <v>0</v>
       </c>
+      <c r="CZ6" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="7" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>1046</v>
       </c>
@@ -5763,8 +5791,11 @@
       <c r="CY7">
         <v>0</v>
       </c>
+      <c r="CZ7" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="8" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>1044</v>
       </c>
@@ -6065,8 +6096,11 @@
       <c r="CY8" t="s">
         <v>23</v>
       </c>
+      <c r="CZ8" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="9" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>1042</v>
       </c>
@@ -6367,8 +6401,11 @@
       <c r="CY9">
         <v>0</v>
       </c>
+      <c r="CZ9" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="10" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>1039</v>
       </c>
@@ -6669,8 +6706,11 @@
       <c r="CY10" t="s">
         <v>0</v>
       </c>
+      <c r="CZ10" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="11" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>1036</v>
       </c>
@@ -6971,8 +7011,11 @@
       <c r="CY11" t="s">
         <v>1033</v>
       </c>
+      <c r="CZ11" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="12" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>1032</v>
       </c>
@@ -7273,8 +7316,11 @@
       <c r="CY12">
         <v>0</v>
       </c>
+      <c r="CZ12" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="13" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>1029</v>
       </c>
@@ -7575,8 +7621,11 @@
       <c r="CY13" t="s">
         <v>133</v>
       </c>
+      <c r="CZ13" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="14" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>1026</v>
       </c>
@@ -7877,8 +7926,11 @@
       <c r="CY14" t="s">
         <v>51</v>
       </c>
+      <c r="CZ14" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="15" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>1024</v>
       </c>
@@ -8179,8 +8231,11 @@
       <c r="CY15" t="s">
         <v>51</v>
       </c>
+      <c r="CZ15" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="16" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>1020</v>
       </c>
@@ -8481,8 +8536,11 @@
       <c r="CY16">
         <v>0</v>
       </c>
+      <c r="CZ16" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="17" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>1018</v>
       </c>
@@ -8783,8 +8841,11 @@
       <c r="CY17">
         <v>0</v>
       </c>
+      <c r="CZ17" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="18" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>1014</v>
       </c>
@@ -9085,8 +9146,11 @@
       <c r="CY18">
         <v>0</v>
       </c>
+      <c r="CZ18" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="19" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>1011</v>
       </c>
@@ -9387,8 +9451,11 @@
       <c r="CY19" t="s">
         <v>104</v>
       </c>
+      <c r="CZ19" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="20" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>1009</v>
       </c>
@@ -9689,8 +9756,11 @@
       <c r="CY20">
         <v>0</v>
       </c>
+      <c r="CZ20" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="21" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>1006</v>
       </c>
@@ -9991,8 +10061,11 @@
       <c r="CY21" t="s">
         <v>1004</v>
       </c>
+      <c r="CZ21" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="22" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>1003</v>
       </c>
@@ -10293,8 +10366,11 @@
       <c r="CY22">
         <v>0</v>
       </c>
+      <c r="CZ22" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="23" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>1001</v>
       </c>
@@ -10595,8 +10671,11 @@
       <c r="CY23" t="s">
         <v>572</v>
       </c>
+      <c r="CZ23" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="24" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>998</v>
       </c>
@@ -10897,8 +10976,11 @@
       <c r="CY24">
         <v>0</v>
       </c>
+      <c r="CZ24" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="25" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>996</v>
       </c>
@@ -11199,8 +11281,11 @@
       <c r="CY25" t="s">
         <v>973</v>
       </c>
+      <c r="CZ25" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="26" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>994</v>
       </c>
@@ -11501,8 +11586,11 @@
       <c r="CY26" t="s">
         <v>22</v>
       </c>
+      <c r="CZ26" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="27" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>991</v>
       </c>
@@ -11803,8 +11891,11 @@
       <c r="CY27" t="s">
         <v>989</v>
       </c>
+      <c r="CZ27" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="28" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>988</v>
       </c>
@@ -12105,8 +12196,11 @@
       <c r="CY28" t="s">
         <v>214</v>
       </c>
+      <c r="CZ28" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="29" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>985</v>
       </c>
@@ -12407,8 +12501,11 @@
       <c r="CY29" t="s">
         <v>982</v>
       </c>
+      <c r="CZ29" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="30" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>981</v>
       </c>
@@ -12709,8 +12806,11 @@
       <c r="CY30" t="s">
         <v>976</v>
       </c>
+      <c r="CZ30" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="31" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>979</v>
       </c>
@@ -13011,8 +13111,11 @@
       <c r="CY31" t="s">
         <v>976</v>
       </c>
+      <c r="CZ31" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="32" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>975</v>
       </c>
@@ -13313,8 +13416,11 @@
       <c r="CY32" t="s">
         <v>972</v>
       </c>
+      <c r="CZ32" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="33" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>971</v>
       </c>
@@ -13615,8 +13721,11 @@
       <c r="CY33" t="s">
         <v>969</v>
       </c>
+      <c r="CZ33" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="34" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>968</v>
       </c>
@@ -13917,8 +14026,11 @@
       <c r="CY34">
         <v>0</v>
       </c>
+      <c r="CZ34" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="35" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>966</v>
       </c>
@@ -14219,8 +14331,11 @@
       <c r="CY35">
         <v>0</v>
       </c>
+      <c r="CZ35" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="36" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>963</v>
       </c>
@@ -14521,8 +14636,11 @@
       <c r="CY36">
         <v>0</v>
       </c>
+      <c r="CZ36" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="37" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>961</v>
       </c>
@@ -14823,8 +14941,11 @@
       <c r="CY37" t="s">
         <v>147</v>
       </c>
+      <c r="CZ37" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="38" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>959</v>
       </c>
@@ -15125,8 +15246,11 @@
       <c r="CY38" t="s">
         <v>623</v>
       </c>
+      <c r="CZ38" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="39" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>956</v>
       </c>
@@ -15427,8 +15551,11 @@
       <c r="CY39" t="s">
         <v>670</v>
       </c>
+      <c r="CZ39" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="40" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>953</v>
       </c>
@@ -15729,8 +15856,11 @@
       <c r="CY40">
         <v>0</v>
       </c>
+      <c r="CZ40" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="41" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>951</v>
       </c>
@@ -16031,8 +16161,11 @@
       <c r="CY41" t="s">
         <v>478</v>
       </c>
+      <c r="CZ41" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="42" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>949</v>
       </c>
@@ -16333,8 +16466,11 @@
       <c r="CY42">
         <v>0</v>
       </c>
+      <c r="CZ42" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="43" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>946</v>
       </c>
@@ -16635,8 +16771,11 @@
       <c r="CY43" t="s">
         <v>670</v>
       </c>
+      <c r="CZ43" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="44" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>943</v>
       </c>
@@ -16937,8 +17076,11 @@
       <c r="CY44" t="s">
         <v>514</v>
       </c>
+      <c r="CZ44" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="45" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>941</v>
       </c>
@@ -17239,8 +17381,11 @@
       <c r="CY45">
         <v>0</v>
       </c>
+      <c r="CZ45" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="46" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>939</v>
       </c>
@@ -17541,8 +17686,11 @@
       <c r="CY46" t="s">
         <v>937</v>
       </c>
+      <c r="CZ46" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="47" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>936</v>
       </c>
@@ -17843,8 +17991,11 @@
       <c r="CY47">
         <v>0</v>
       </c>
+      <c r="CZ47" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="48" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>934</v>
       </c>
@@ -18145,8 +18296,11 @@
       <c r="CY48" t="s">
         <v>932</v>
       </c>
+      <c r="CZ48" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="49" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>931</v>
       </c>
@@ -18447,8 +18601,11 @@
       <c r="CY49" t="s">
         <v>929</v>
       </c>
+      <c r="CZ49" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="50" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>928</v>
       </c>
@@ -18749,8 +18906,11 @@
       <c r="CY50" t="s">
         <v>22</v>
       </c>
+      <c r="CZ50" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="51" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>925</v>
       </c>
@@ -19051,8 +19211,11 @@
       <c r="CY51" t="s">
         <v>51</v>
       </c>
+      <c r="CZ51" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="52" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>923</v>
       </c>
@@ -19353,8 +19516,11 @@
       <c r="CY52" t="s">
         <v>920</v>
       </c>
+      <c r="CZ52" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="53" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>919</v>
       </c>
@@ -19655,8 +19821,11 @@
       <c r="CY53" t="s">
         <v>22</v>
       </c>
+      <c r="CZ53" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="54" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>916</v>
       </c>
@@ -19957,8 +20126,11 @@
       <c r="CY54">
         <v>0</v>
       </c>
+      <c r="CZ54" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="55" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>914</v>
       </c>
@@ -20259,8 +20431,11 @@
       <c r="CY55" t="s">
         <v>511</v>
       </c>
+      <c r="CZ55" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="56" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>912</v>
       </c>
@@ -20561,8 +20736,11 @@
       <c r="CY56" t="s">
         <v>51</v>
       </c>
+      <c r="CZ56" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="57" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>910</v>
       </c>
@@ -20863,8 +21041,11 @@
       <c r="CY57">
         <v>0</v>
       </c>
+      <c r="CZ57" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="58" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>907</v>
       </c>
@@ -21165,8 +21346,11 @@
       <c r="CY58">
         <v>0</v>
       </c>
+      <c r="CZ58" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="59" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>904</v>
       </c>
@@ -21467,8 +21651,11 @@
       <c r="CY59" t="s">
         <v>902</v>
       </c>
+      <c r="CZ59" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="60" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>901</v>
       </c>
@@ -21769,8 +21956,11 @@
       <c r="CY60" t="s">
         <v>727</v>
       </c>
+      <c r="CZ60" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="61" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>898</v>
       </c>
@@ -22071,8 +22261,11 @@
       <c r="CY61" t="s">
         <v>23</v>
       </c>
+      <c r="CZ61" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="62" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>895</v>
       </c>
@@ -22373,8 +22566,11 @@
       <c r="CY62" t="s">
         <v>893</v>
       </c>
+      <c r="CZ62" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="63" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>892</v>
       </c>
@@ -22675,8 +22871,11 @@
       <c r="CY63" t="s">
         <v>678</v>
       </c>
+      <c r="CZ63" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="64" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>889</v>
       </c>
@@ -22977,8 +23176,11 @@
       <c r="CY64" t="s">
         <v>887</v>
       </c>
+      <c r="CZ64" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="65" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>886</v>
       </c>
@@ -23279,8 +23481,11 @@
       <c r="CY65" t="s">
         <v>147</v>
       </c>
+      <c r="CZ65" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="66" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>884</v>
       </c>
@@ -23581,8 +23786,11 @@
       <c r="CY66">
         <v>0</v>
       </c>
+      <c r="CZ66" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="67" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>881</v>
       </c>
@@ -23883,8 +24091,11 @@
       <c r="CY67" t="s">
         <v>51</v>
       </c>
+      <c r="CZ67" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="68" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>878</v>
       </c>
@@ -24185,8 +24396,11 @@
       <c r="CY68" t="s">
         <v>876</v>
       </c>
+      <c r="CZ68" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="69" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>875</v>
       </c>
@@ -24487,8 +24701,11 @@
       <c r="CY69" t="s">
         <v>97</v>
       </c>
+      <c r="CZ69" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="70" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>873</v>
       </c>
@@ -24789,8 +25006,11 @@
       <c r="CY70" t="s">
         <v>291</v>
       </c>
+      <c r="CZ70" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="71" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>871</v>
       </c>
@@ -25091,8 +25311,11 @@
       <c r="CY71" t="s">
         <v>511</v>
       </c>
+      <c r="CZ71" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="72" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>869</v>
       </c>
@@ -25393,8 +25616,11 @@
       <c r="CY72" t="s">
         <v>46</v>
       </c>
+      <c r="CZ72" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="73" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>866</v>
       </c>
@@ -25695,8 +25921,11 @@
       <c r="CY73" t="s">
         <v>31</v>
       </c>
+      <c r="CZ73" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="74" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>864</v>
       </c>
@@ -25997,8 +26226,11 @@
       <c r="CY74" t="s">
         <v>817</v>
       </c>
+      <c r="CZ74" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="75" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>861</v>
       </c>
@@ -26299,8 +26531,11 @@
       <c r="CY75" t="s">
         <v>256</v>
       </c>
+      <c r="CZ75" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="76" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>857</v>
       </c>
@@ -26601,8 +26836,11 @@
       <c r="CY76" t="s">
         <v>855</v>
       </c>
+      <c r="CZ76" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="77" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>854</v>
       </c>
@@ -26903,8 +27141,11 @@
       <c r="CY77" t="s">
         <v>851</v>
       </c>
+      <c r="CZ77" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="78" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>850</v>
       </c>
@@ -27205,8 +27446,11 @@
       <c r="CY78">
         <v>0</v>
       </c>
+      <c r="CZ78" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="79" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>848</v>
       </c>
@@ -27507,8 +27751,11 @@
       <c r="CY79" t="s">
         <v>37</v>
       </c>
+      <c r="CZ79" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="80" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>845</v>
       </c>
@@ -27809,8 +28056,11 @@
       <c r="CY80">
         <v>0</v>
       </c>
+      <c r="CZ80" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="81" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>843</v>
       </c>
@@ -28111,8 +28361,11 @@
       <c r="CY81" t="s">
         <v>147</v>
       </c>
+      <c r="CZ81" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="82" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>841</v>
       </c>
@@ -28413,8 +28666,11 @@
       <c r="CY82" t="s">
         <v>51</v>
       </c>
+      <c r="CZ82" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="83" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>839</v>
       </c>
@@ -28715,8 +28971,11 @@
       <c r="CY83">
         <v>0</v>
       </c>
+      <c r="CZ83" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="84" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>837</v>
       </c>
@@ -29017,8 +29276,11 @@
       <c r="CY84" t="s">
         <v>97</v>
       </c>
+      <c r="CZ84" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="85" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>835</v>
       </c>
@@ -29319,8 +29581,11 @@
       <c r="CY85">
         <v>0</v>
       </c>
+      <c r="CZ85" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="86" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>833</v>
       </c>
@@ -29621,8 +29886,11 @@
       <c r="CY86" t="s">
         <v>230</v>
       </c>
+      <c r="CZ86" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="87" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>830</v>
       </c>
@@ -29923,8 +30191,11 @@
       <c r="CY87">
         <v>0</v>
       </c>
+      <c r="CZ87" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="88" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>827</v>
       </c>
@@ -30225,8 +30496,11 @@
       <c r="CY88" t="s">
         <v>51</v>
       </c>
+      <c r="CZ88" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="89" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>824</v>
       </c>
@@ -30527,8 +30801,11 @@
       <c r="CY89" t="s">
         <v>51</v>
       </c>
+      <c r="CZ89" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="90" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>821</v>
       </c>
@@ -30829,8 +31106,11 @@
       <c r="CY90">
         <v>0</v>
       </c>
+      <c r="CZ90" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="91" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>819</v>
       </c>
@@ -31131,8 +31411,11 @@
       <c r="CY91" t="s">
         <v>97</v>
       </c>
+      <c r="CZ91" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="92" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>816</v>
       </c>
@@ -31433,8 +31716,11 @@
       <c r="CY92" t="s">
         <v>291</v>
       </c>
+      <c r="CZ92" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="93" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>813</v>
       </c>
@@ -31735,8 +32021,11 @@
       <c r="CY93" t="s">
         <v>811</v>
       </c>
+      <c r="CZ93" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="94" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>810</v>
       </c>
@@ -32037,8 +32326,11 @@
       <c r="CY94">
         <v>0</v>
       </c>
+      <c r="CZ94" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="95" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>807</v>
       </c>
@@ -32339,8 +32631,11 @@
       <c r="CY95" t="s">
         <v>249</v>
       </c>
+      <c r="CZ95" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="96" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>804</v>
       </c>
@@ -32641,8 +32936,11 @@
       <c r="CY96" t="s">
         <v>22</v>
       </c>
+      <c r="CZ96" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="97" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>801</v>
       </c>
@@ -32943,8 +33241,11 @@
       <c r="CY97">
         <v>0</v>
       </c>
+      <c r="CZ97" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="98" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>799</v>
       </c>
@@ -33245,8 +33546,11 @@
       <c r="CY98" t="s">
         <v>23</v>
       </c>
+      <c r="CZ98" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="99" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>796</v>
       </c>
@@ -33547,8 +33851,11 @@
       <c r="CY99" t="s">
         <v>654</v>
       </c>
+      <c r="CZ99" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="100" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>794</v>
       </c>
@@ -33849,8 +34156,11 @@
       <c r="CY100" t="s">
         <v>791</v>
       </c>
+      <c r="CZ100" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="101" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>790</v>
       </c>
@@ -34151,8 +34461,11 @@
       <c r="CY101" t="s">
         <v>147</v>
       </c>
+      <c r="CZ101" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="102" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>788</v>
       </c>
@@ -34453,8 +34766,11 @@
       <c r="CY102">
         <v>0</v>
       </c>
+      <c r="CZ102" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="103" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>786</v>
       </c>
@@ -34755,8 +35071,11 @@
       <c r="CY103" t="s">
         <v>23</v>
       </c>
+      <c r="CZ103" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="104" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>783</v>
       </c>
@@ -35057,8 +35376,11 @@
       <c r="CY104" t="s">
         <v>739</v>
       </c>
+      <c r="CZ104" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="105" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>780</v>
       </c>
@@ -35359,8 +35681,11 @@
       <c r="CY105">
         <v>0</v>
       </c>
+      <c r="CZ105" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="106" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>776</v>
       </c>
@@ -35661,8 +35986,11 @@
       <c r="CY106">
         <v>0</v>
       </c>
+      <c r="CZ106" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="107" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>774</v>
       </c>
@@ -35963,8 +36291,11 @@
       <c r="CY107" t="s">
         <v>771</v>
       </c>
+      <c r="CZ107" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="108" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>770</v>
       </c>
@@ -36265,8 +36596,11 @@
       <c r="CY108" t="s">
         <v>768</v>
       </c>
+      <c r="CZ108" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="109" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>767</v>
       </c>
@@ -36567,8 +36901,11 @@
       <c r="CY109" t="s">
         <v>308</v>
       </c>
+      <c r="CZ109" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="110" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>764</v>
       </c>
@@ -36869,8 +37206,11 @@
       <c r="CY110">
         <v>0</v>
       </c>
+      <c r="CZ110" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="111" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>761</v>
       </c>
@@ -37171,8 +37511,11 @@
       <c r="CY111" t="s">
         <v>338</v>
       </c>
+      <c r="CZ111" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="112" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>758</v>
       </c>
@@ -37473,8 +37816,11 @@
       <c r="CY112" t="s">
         <v>755</v>
       </c>
+      <c r="CZ112" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="113" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>754</v>
       </c>
@@ -37775,8 +38121,11 @@
       <c r="CY113" t="s">
         <v>147</v>
       </c>
+      <c r="CZ113" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="114" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>751</v>
       </c>
@@ -38077,8 +38426,11 @@
       <c r="CY114" t="s">
         <v>23</v>
       </c>
+      <c r="CZ114" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="115" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>749</v>
       </c>
@@ -38379,8 +38731,11 @@
       <c r="CY115" t="s">
         <v>22</v>
       </c>
+      <c r="CZ115" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="116" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>746</v>
       </c>
@@ -38681,8 +39036,11 @@
       <c r="CY116">
         <v>0</v>
       </c>
+      <c r="CZ116" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="117" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>744</v>
       </c>
@@ -38983,8 +39341,11 @@
       <c r="CY117" t="s">
         <v>51</v>
       </c>
+      <c r="CZ117" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="118" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>741</v>
       </c>
@@ -39285,8 +39646,11 @@
       <c r="CY118" t="s">
         <v>739</v>
       </c>
+      <c r="CZ118" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="119" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>738</v>
       </c>
@@ -39587,8 +39951,11 @@
       <c r="CY119" t="s">
         <v>475</v>
       </c>
+      <c r="CZ119" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="120" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>735</v>
       </c>
@@ -39889,8 +40256,11 @@
       <c r="CY120" t="s">
         <v>51</v>
       </c>
+      <c r="CZ120" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="121" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>733</v>
       </c>
@@ -40191,8 +40561,11 @@
       <c r="CY121" t="s">
         <v>22</v>
       </c>
+      <c r="CZ121" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="122" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>730</v>
       </c>
@@ -40493,8 +40866,11 @@
       <c r="CY122" t="s">
         <v>727</v>
       </c>
+      <c r="CZ122" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="123" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>726</v>
       </c>
@@ -40795,8 +41171,11 @@
       <c r="CY123" t="s">
         <v>147</v>
       </c>
+      <c r="CZ123" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="124" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>724</v>
       </c>
@@ -41097,8 +41476,11 @@
       <c r="CY124" t="s">
         <v>721</v>
       </c>
+      <c r="CZ124" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="125" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>720</v>
       </c>
@@ -41399,8 +41781,11 @@
       <c r="CY125">
         <v>0</v>
       </c>
+      <c r="CZ125" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="126" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>718</v>
       </c>
@@ -41701,8 +42086,11 @@
       <c r="CY126" t="s">
         <v>22</v>
       </c>
+      <c r="CZ126" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="127" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>716</v>
       </c>
@@ -42003,8 +42391,11 @@
       <c r="CY127" t="s">
         <v>662</v>
       </c>
+      <c r="CZ127" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="128" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>714</v>
       </c>
@@ -42305,8 +42696,11 @@
       <c r="CY128" t="s">
         <v>22</v>
       </c>
+      <c r="CZ128" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="129" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>712</v>
       </c>
@@ -42607,8 +43001,11 @@
       <c r="CY129">
         <v>0</v>
       </c>
+      <c r="CZ129" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="130" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>709</v>
       </c>
@@ -42909,8 +43306,11 @@
       <c r="CY130">
         <v>0</v>
       </c>
+      <c r="CZ130" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="131" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>706</v>
       </c>
@@ -43211,8 +43611,11 @@
       <c r="CY131" t="s">
         <v>22</v>
       </c>
+      <c r="CZ131" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="132" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>702</v>
       </c>
@@ -43513,8 +43916,11 @@
       <c r="CY132" t="s">
         <v>699</v>
       </c>
+      <c r="CZ132" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="133" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>698</v>
       </c>
@@ -43815,8 +44221,11 @@
       <c r="CY133" t="s">
         <v>379</v>
       </c>
+      <c r="CZ133" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="134" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>695</v>
       </c>
@@ -44117,8 +44526,11 @@
       <c r="CY134" t="s">
         <v>219</v>
       </c>
+      <c r="CZ134" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="135" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>693</v>
       </c>
@@ -44419,8 +44831,11 @@
       <c r="CY135" t="s">
         <v>46</v>
       </c>
+      <c r="CZ135" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="136" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>691</v>
       </c>
@@ -44721,8 +45136,11 @@
       <c r="CY136">
         <v>0</v>
       </c>
+      <c r="CZ136" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="137" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>688</v>
       </c>
@@ -45023,8 +45441,11 @@
       <c r="CY137" t="s">
         <v>390</v>
       </c>
+      <c r="CZ137" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="138" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>686</v>
       </c>
@@ -45325,8 +45746,11 @@
       <c r="CY138" t="s">
         <v>682</v>
       </c>
+      <c r="CZ138" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="139" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>681</v>
       </c>
@@ -45627,8 +46051,11 @@
       <c r="CY139" t="s">
         <v>23</v>
       </c>
+      <c r="CZ139" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="140" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>677</v>
       </c>
@@ -45929,8 +46356,11 @@
       <c r="CY140">
         <v>0</v>
       </c>
+      <c r="CZ140" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="141" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>673</v>
       </c>
@@ -46231,8 +46661,11 @@
       <c r="CY141" t="s">
         <v>670</v>
       </c>
+      <c r="CZ141" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="142" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>669</v>
       </c>
@@ -46533,8 +46966,11 @@
       <c r="CY142" t="s">
         <v>667</v>
       </c>
+      <c r="CZ142" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="143" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>666</v>
       </c>
@@ -46835,8 +47271,11 @@
       <c r="CY143" t="s">
         <v>662</v>
       </c>
+      <c r="CZ143" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="144" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>661</v>
       </c>
@@ -47137,8 +47576,11 @@
       <c r="CY144" t="s">
         <v>104</v>
       </c>
+      <c r="CZ144" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="145" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>659</v>
       </c>
@@ -47439,8 +47881,11 @@
       <c r="CY145">
         <v>0</v>
       </c>
+      <c r="CZ145" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="146" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>657</v>
       </c>
@@ -47741,8 +48186,11 @@
       <c r="CY146" t="s">
         <v>249</v>
       </c>
+      <c r="CZ146" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="147" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>653</v>
       </c>
@@ -48043,8 +48491,11 @@
       <c r="CY147">
         <v>0</v>
       </c>
+      <c r="CZ147" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="148" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>651</v>
       </c>
@@ -48345,8 +48796,11 @@
       <c r="CY148">
         <v>0</v>
       </c>
+      <c r="CZ148" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="149" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>648</v>
       </c>
@@ -48647,8 +49101,11 @@
       <c r="CY149" t="s">
         <v>646</v>
       </c>
+      <c r="CZ149" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="150" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>645</v>
       </c>
@@ -48949,8 +49406,11 @@
       <c r="CY150" t="s">
         <v>643</v>
       </c>
+      <c r="CZ150" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="151" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>642</v>
       </c>
@@ -49251,8 +49711,11 @@
       <c r="CY151" t="s">
         <v>0</v>
       </c>
+      <c r="CZ151" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="152" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>640</v>
       </c>
@@ -49553,8 +50016,11 @@
       <c r="CY152" t="s">
         <v>51</v>
       </c>
+      <c r="CZ152" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="153" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>636</v>
       </c>
@@ -49855,8 +50321,11 @@
       <c r="CY153" t="s">
         <v>22</v>
       </c>
+      <c r="CZ153" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="154" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>633</v>
       </c>
@@ -50157,8 +50626,11 @@
       <c r="CY154" t="s">
         <v>97</v>
       </c>
+      <c r="CZ154" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="155" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>630</v>
       </c>
@@ -50459,8 +50931,11 @@
       <c r="CY155" t="s">
         <v>147</v>
       </c>
+      <c r="CZ155" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="156" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>627</v>
       </c>
@@ -50761,8 +51236,11 @@
       <c r="CY156" t="s">
         <v>110</v>
       </c>
+      <c r="CZ156" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="157" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>625</v>
       </c>
@@ -51063,8 +51541,11 @@
       <c r="CY157">
         <v>0</v>
       </c>
+      <c r="CZ157" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="158" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>622</v>
       </c>
@@ -51365,8 +51846,11 @@
       <c r="CY158">
         <v>0</v>
       </c>
+      <c r="CZ158" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="159" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>618</v>
       </c>
@@ -51667,8 +52151,11 @@
       <c r="CY159" t="s">
         <v>615</v>
       </c>
+      <c r="CZ159" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="160" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>614</v>
       </c>
@@ -51969,8 +52456,11 @@
       <c r="CY160" t="s">
         <v>611</v>
       </c>
+      <c r="CZ160" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="161" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>610</v>
       </c>
@@ -52271,8 +52761,11 @@
       <c r="CY161" t="s">
         <v>104</v>
       </c>
+      <c r="CZ161" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="162" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>608</v>
       </c>
@@ -52573,8 +53066,11 @@
       <c r="CY162" t="s">
         <v>604</v>
       </c>
+      <c r="CZ162" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="163" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>603</v>
       </c>
@@ -52875,8 +53371,11 @@
       <c r="CY163">
         <v>0</v>
       </c>
+      <c r="CZ163" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="164" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>600</v>
       </c>
@@ -53177,8 +53676,11 @@
       <c r="CY164" t="s">
         <v>22</v>
       </c>
+      <c r="CZ164" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="165" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>598</v>
       </c>
@@ -53479,8 +53981,11 @@
       <c r="CY165">
         <v>0</v>
       </c>
+      <c r="CZ165" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="166" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>596</v>
       </c>
@@ -53781,8 +54286,11 @@
       <c r="CY166" t="s">
         <v>51</v>
       </c>
+      <c r="CZ166" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="167" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>593</v>
       </c>
@@ -54083,8 +54591,11 @@
       <c r="CY167" t="s">
         <v>22</v>
       </c>
+      <c r="CZ167" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="168" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>590</v>
       </c>
@@ -54385,8 +54896,11 @@
       <c r="CY168">
         <v>0</v>
       </c>
+      <c r="CZ168" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="169" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>587</v>
       </c>
@@ -54687,8 +55201,11 @@
       <c r="CY169" t="s">
         <v>154</v>
       </c>
+      <c r="CZ169" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="170" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>582</v>
       </c>
@@ -54989,8 +55506,11 @@
       <c r="CY170" t="s">
         <v>51</v>
       </c>
+      <c r="CZ170" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="171" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>580</v>
       </c>
@@ -55291,8 +55811,11 @@
       <c r="CY171" t="s">
         <v>249</v>
       </c>
+      <c r="CZ171" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="172" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>577</v>
       </c>
@@ -55593,8 +56116,11 @@
       <c r="CY172">
         <v>0</v>
       </c>
+      <c r="CZ172" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="173" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>574</v>
       </c>
@@ -55895,8 +56421,11 @@
       <c r="CY173" t="s">
         <v>309</v>
       </c>
+      <c r="CZ173" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="174" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>571</v>
       </c>
@@ -56197,8 +56726,11 @@
       <c r="CY174" t="s">
         <v>23</v>
       </c>
+      <c r="CZ174" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="175" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>568</v>
       </c>
@@ -56499,8 +57031,11 @@
       <c r="CY175">
         <v>0</v>
       </c>
+      <c r="CZ175" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="176" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>565</v>
       </c>
@@ -56801,8 +57336,11 @@
       <c r="CY176" t="s">
         <v>22</v>
       </c>
+      <c r="CZ176" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="177" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>562</v>
       </c>
@@ -57103,8 +57641,11 @@
       <c r="CY177">
         <v>0</v>
       </c>
+      <c r="CZ177" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="178" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>559</v>
       </c>
@@ -57405,8 +57946,11 @@
       <c r="CY178">
         <v>0</v>
       </c>
+      <c r="CZ178" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="179" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>556</v>
       </c>
@@ -57707,8 +58251,11 @@
       <c r="CY179">
         <v>0</v>
       </c>
+      <c r="CZ179" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="180" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>553</v>
       </c>
@@ -58009,8 +58556,11 @@
       <c r="CY180" t="s">
         <v>23</v>
       </c>
+      <c r="CZ180" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="181" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>551</v>
       </c>
@@ -58311,8 +58861,11 @@
       <c r="CY181" t="s">
         <v>549</v>
       </c>
+      <c r="CZ181" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="182" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>548</v>
       </c>
@@ -58613,8 +59166,11 @@
       <c r="CY182">
         <v>0</v>
       </c>
+      <c r="CZ182" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="183" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>545</v>
       </c>
@@ -58915,8 +59471,11 @@
       <c r="CY183" t="s">
         <v>22</v>
       </c>
+      <c r="CZ183" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="184" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>542</v>
       </c>
@@ -59217,8 +59776,11 @@
       <c r="CY184" t="s">
         <v>23</v>
       </c>
+      <c r="CZ184" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="185" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>540</v>
       </c>
@@ -59519,8 +60081,11 @@
       <c r="CY185" t="s">
         <v>537</v>
       </c>
+      <c r="CZ185" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="186" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>536</v>
       </c>
@@ -59821,8 +60386,11 @@
       <c r="CY186" t="s">
         <v>532</v>
       </c>
+      <c r="CZ186" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="187" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>531</v>
       </c>
@@ -60123,8 +60691,11 @@
       <c r="CY187" t="s">
         <v>387</v>
       </c>
+      <c r="CZ187" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="188" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>529</v>
       </c>
@@ -60425,8 +60996,11 @@
       <c r="CY188" t="s">
         <v>22</v>
       </c>
+      <c r="CZ188" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="189" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>526</v>
       </c>
@@ -60727,8 +61301,11 @@
       <c r="CY189" t="s">
         <v>514</v>
       </c>
+      <c r="CZ189" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="190" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>523</v>
       </c>
@@ -61029,8 +61606,11 @@
       <c r="CY190">
         <v>0</v>
       </c>
+      <c r="CZ190" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="191" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>519</v>
       </c>
@@ -61331,8 +61911,11 @@
       <c r="CY191">
         <v>0</v>
       </c>
+      <c r="CZ191" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="192" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>517</v>
       </c>
@@ -61633,8 +62216,11 @@
       <c r="CY192">
         <v>0</v>
       </c>
+      <c r="CZ192" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="193" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>513</v>
       </c>
@@ -61935,8 +62521,11 @@
       <c r="CY193" t="s">
         <v>23</v>
       </c>
+      <c r="CZ193" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="194" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>510</v>
       </c>
@@ -62237,8 +62826,11 @@
       <c r="CY194" t="s">
         <v>51</v>
       </c>
+      <c r="CZ194" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="195" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>507</v>
       </c>
@@ -62539,8 +63131,11 @@
       <c r="CY195">
         <v>0</v>
       </c>
+      <c r="CZ195" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="196" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>505</v>
       </c>
@@ -62841,8 +63436,11 @@
       <c r="CY196">
         <v>0</v>
       </c>
+      <c r="CZ196" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="197" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>502</v>
       </c>
@@ -63143,8 +63741,11 @@
       <c r="CY197" t="s">
         <v>16</v>
       </c>
+      <c r="CZ197" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="198" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>498</v>
       </c>
@@ -63445,8 +64046,11 @@
       <c r="CY198" t="s">
         <v>438</v>
       </c>
+      <c r="CZ198" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="199" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>495</v>
       </c>
@@ -63747,8 +64351,11 @@
       <c r="CY199">
         <v>0</v>
       </c>
+      <c r="CZ199" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="200" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>493</v>
       </c>
@@ -64049,8 +64656,11 @@
       <c r="CY200">
         <v>0</v>
       </c>
+      <c r="CZ200" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="201" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>490</v>
       </c>
@@ -64351,8 +64961,11 @@
       <c r="CY201">
         <v>0</v>
       </c>
+      <c r="CZ201" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="202" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>486</v>
       </c>
@@ -64653,8 +65266,11 @@
       <c r="CY202" t="s">
         <v>97</v>
       </c>
+      <c r="CZ202" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="203" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>484</v>
       </c>
@@ -64955,8 +65571,11 @@
       <c r="CY203" t="s">
         <v>426</v>
       </c>
+      <c r="CZ203" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="204" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>482</v>
       </c>
@@ -65257,8 +65876,11 @@
       <c r="CY204" t="s">
         <v>478</v>
       </c>
+      <c r="CZ204" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="205" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>477</v>
       </c>
@@ -65559,8 +66181,11 @@
       <c r="CY205">
         <v>0</v>
       </c>
+      <c r="CZ205" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="206" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>474</v>
       </c>
@@ -65861,8 +66486,11 @@
       <c r="CY206" t="s">
         <v>23</v>
       </c>
+      <c r="CZ206" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="207" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>471</v>
       </c>
@@ -66163,8 +66791,11 @@
       <c r="CY207" t="s">
         <v>147</v>
       </c>
+      <c r="CZ207" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="208" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>468</v>
       </c>
@@ -66465,8 +67096,11 @@
       <c r="CY208" t="s">
         <v>23</v>
       </c>
+      <c r="CZ208" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="209" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>465</v>
       </c>
@@ -66767,8 +67401,11 @@
       <c r="CY209" t="s">
         <v>23</v>
       </c>
+      <c r="CZ209" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="210" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>462</v>
       </c>
@@ -67069,8 +67706,11 @@
       <c r="CY210">
         <v>0</v>
       </c>
+      <c r="CZ210" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="211" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>460</v>
       </c>
@@ -67371,8 +68011,11 @@
       <c r="CY211" t="s">
         <v>51</v>
       </c>
+      <c r="CZ211" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="212" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>458</v>
       </c>
@@ -67673,8 +68316,11 @@
       <c r="CY212">
         <v>0</v>
       </c>
+      <c r="CZ212" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="213" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>456</v>
       </c>
@@ -67975,8 +68621,11 @@
       <c r="CY213" t="s">
         <v>454</v>
       </c>
+      <c r="CZ213" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="214" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>453</v>
       </c>
@@ -68277,8 +68926,11 @@
       <c r="CY214" t="s">
         <v>70</v>
       </c>
+      <c r="CZ214" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="215" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>450</v>
       </c>
@@ -68579,8 +69231,11 @@
       <c r="CY215" t="s">
         <v>51</v>
       </c>
+      <c r="CZ215" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="216" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>447</v>
       </c>
@@ -68881,8 +69536,11 @@
       <c r="CY216">
         <v>0</v>
       </c>
+      <c r="CZ216" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="217" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>445</v>
       </c>
@@ -69183,8 +69841,11 @@
       <c r="CY217" t="s">
         <v>442</v>
       </c>
+      <c r="CZ217" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="218" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>441</v>
       </c>
@@ -69485,8 +70146,11 @@
       <c r="CY218" t="s">
         <v>437</v>
       </c>
+      <c r="CZ218" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="219" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>436</v>
       </c>
@@ -69787,8 +70451,11 @@
       <c r="CY219" t="s">
         <v>22</v>
       </c>
+      <c r="CZ219" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="220" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>433</v>
       </c>
@@ -70089,8 +70756,11 @@
       <c r="CY220">
         <v>0</v>
       </c>
+      <c r="CZ220" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="221" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>429</v>
       </c>
@@ -70391,8 +71061,11 @@
       <c r="CY221" t="s">
         <v>51</v>
       </c>
+      <c r="CZ221" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="222" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>425</v>
       </c>
@@ -70693,8 +71366,11 @@
       <c r="CY222">
         <v>0</v>
       </c>
+      <c r="CZ222" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="223" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>422</v>
       </c>
@@ -70995,8 +71671,11 @@
       <c r="CY223" t="s">
         <v>51</v>
       </c>
+      <c r="CZ223" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="224" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>420</v>
       </c>
@@ -71297,8 +71976,11 @@
       <c r="CY224" t="s">
         <v>119</v>
       </c>
+      <c r="CZ224" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="225" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>417</v>
       </c>
@@ -71599,8 +72281,11 @@
       <c r="CY225">
         <v>0</v>
       </c>
+      <c r="CZ225" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="226" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>414</v>
       </c>
@@ -71901,8 +72586,11 @@
       <c r="CY226" t="s">
         <v>51</v>
       </c>
+      <c r="CZ226" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="227" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>411</v>
       </c>
@@ -72203,8 +72891,11 @@
       <c r="CY227" t="s">
         <v>22</v>
       </c>
+      <c r="CZ227" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="228" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>408</v>
       </c>
@@ -72505,8 +73196,11 @@
       <c r="CY228" t="s">
         <v>308</v>
       </c>
+      <c r="CZ228" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="229" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>405</v>
       </c>
@@ -72807,8 +73501,11 @@
       <c r="CY229">
         <v>0</v>
       </c>
+      <c r="CZ229" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="230" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>403</v>
       </c>
@@ -73109,8 +73806,11 @@
       <c r="CY230" t="s">
         <v>400</v>
       </c>
+      <c r="CZ230" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="231" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>399</v>
       </c>
@@ -73411,8 +74111,11 @@
       <c r="CY231">
         <v>0</v>
       </c>
+      <c r="CZ231" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="232" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>396</v>
       </c>
@@ -73713,8 +74416,11 @@
       <c r="CY232">
         <v>0</v>
       </c>
+      <c r="CZ232" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="233" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>393</v>
       </c>
@@ -74015,8 +74721,11 @@
       <c r="CY233" t="s">
         <v>390</v>
       </c>
+      <c r="CZ233" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="234" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>389</v>
       </c>
@@ -74317,8 +75026,11 @@
       <c r="CY234" t="s">
         <v>23</v>
       </c>
+      <c r="CZ234" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="235" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>386</v>
       </c>
@@ -74619,8 +75331,11 @@
       <c r="CY235" t="s">
         <v>147</v>
       </c>
+      <c r="CZ235" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="236" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>382</v>
       </c>
@@ -74921,8 +75636,11 @@
       <c r="CY236" t="s">
         <v>378</v>
       </c>
+      <c r="CZ236" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="237" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>377</v>
       </c>
@@ -75223,8 +75941,11 @@
       <c r="CY237" t="s">
         <v>23</v>
       </c>
+      <c r="CZ237" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="238" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>375</v>
       </c>
@@ -75525,8 +76246,11 @@
       <c r="CY238" t="s">
         <v>51</v>
       </c>
+      <c r="CZ238" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="239" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>372</v>
       </c>
@@ -75827,8 +76551,11 @@
       <c r="CY239">
         <v>0</v>
       </c>
+      <c r="CZ239" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="240" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>368</v>
       </c>
@@ -76129,8 +76856,11 @@
       <c r="CY240" t="s">
         <v>133</v>
       </c>
+      <c r="CZ240" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="241" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>365</v>
       </c>
@@ -76431,8 +77161,11 @@
       <c r="CY241" t="s">
         <v>97</v>
       </c>
+      <c r="CZ241" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="242" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>363</v>
       </c>
@@ -76733,8 +77466,11 @@
       <c r="CY242" t="s">
         <v>358</v>
       </c>
+      <c r="CZ242" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="243" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>357</v>
       </c>
@@ -77035,8 +77771,11 @@
       <c r="CY243">
         <v>0</v>
       </c>
+      <c r="CZ243" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="244" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>353</v>
       </c>
@@ -77337,8 +78076,11 @@
       <c r="CY244" t="s">
         <v>22</v>
       </c>
+      <c r="CZ244" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="245" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>350</v>
       </c>
@@ -77639,8 +78381,11 @@
       <c r="CY245" t="s">
         <v>133</v>
       </c>
+      <c r="CZ245" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="246" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>347</v>
       </c>
@@ -77941,8 +78686,11 @@
       <c r="CY246" t="s">
         <v>345</v>
       </c>
+      <c r="CZ246" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="247" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>344</v>
       </c>
@@ -78243,8 +78991,11 @@
       <c r="CY247">
         <v>0</v>
       </c>
+      <c r="CZ247" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="248" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>341</v>
       </c>
@@ -78545,8 +79296,11 @@
       <c r="CY248" t="s">
         <v>338</v>
       </c>
+      <c r="CZ248" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="249" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>337</v>
       </c>
@@ -78847,8 +79601,11 @@
       <c r="CY249" t="s">
         <v>23</v>
       </c>
+      <c r="CZ249" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="250" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>334</v>
       </c>
@@ -79149,8 +79906,11 @@
       <c r="CY250" t="s">
         <v>331</v>
       </c>
+      <c r="CZ250" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="251" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>330</v>
       </c>
@@ -79451,8 +80211,11 @@
       <c r="CY251" t="s">
         <v>51</v>
       </c>
+      <c r="CZ251" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="252" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>327</v>
       </c>
@@ -79753,8 +80516,11 @@
       <c r="CY252" t="s">
         <v>324</v>
       </c>
+      <c r="CZ252" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="253" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>323</v>
       </c>
@@ -80055,8 +80821,11 @@
       <c r="CY253">
         <v>0</v>
       </c>
+      <c r="CZ253" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="254" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>321</v>
       </c>
@@ -80357,8 +81126,11 @@
       <c r="CY254" t="s">
         <v>23</v>
       </c>
+      <c r="CZ254" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="255" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>319</v>
       </c>
@@ -80659,8 +81431,11 @@
       <c r="CY255">
         <v>0</v>
       </c>
+      <c r="CZ255" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="256" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>316</v>
       </c>
@@ -80961,8 +81736,11 @@
       <c r="CY256" t="s">
         <v>22</v>
       </c>
+      <c r="CZ256" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="257" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>312</v>
       </c>
@@ -81263,8 +82041,11 @@
       <c r="CY257" t="s">
         <v>308</v>
       </c>
+      <c r="CZ257" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="258" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>307</v>
       </c>
@@ -81565,8 +82346,11 @@
       <c r="CY258" t="s">
         <v>303</v>
       </c>
+      <c r="CZ258" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="259" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>302</v>
       </c>
@@ -81867,8 +82651,11 @@
       <c r="CY259" t="s">
         <v>299</v>
       </c>
+      <c r="CZ259" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="260" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>298</v>
       </c>
@@ -82169,8 +82956,11 @@
       <c r="CY260" t="s">
         <v>295</v>
       </c>
+      <c r="CZ260" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="261" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>294</v>
       </c>
@@ -82471,8 +83261,11 @@
       <c r="CY261" t="s">
         <v>291</v>
       </c>
+      <c r="CZ261" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="262" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>290</v>
       </c>
@@ -82773,8 +83566,11 @@
       <c r="CY262" t="s">
         <v>70</v>
       </c>
+      <c r="CZ262" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="263" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>288</v>
       </c>
@@ -83075,8 +83871,11 @@
       <c r="CY263" t="s">
         <v>282</v>
       </c>
+      <c r="CZ263" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="264" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>281</v>
       </c>
@@ -83377,8 +84176,11 @@
       <c r="CY264" t="s">
         <v>51</v>
       </c>
+      <c r="CZ264" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="265" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>278</v>
       </c>
@@ -83679,8 +84481,11 @@
       <c r="CY265" t="s">
         <v>83</v>
       </c>
+      <c r="CZ265" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="266" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>275</v>
       </c>
@@ -83981,8 +84786,11 @@
       <c r="CY266">
         <v>0</v>
       </c>
+      <c r="CZ266" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="267" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>273</v>
       </c>
@@ -84283,8 +85091,11 @@
       <c r="CY267" t="s">
         <v>51</v>
       </c>
+      <c r="CZ267" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="268" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>270</v>
       </c>
@@ -84585,8 +85396,11 @@
       <c r="CY268" t="s">
         <v>23</v>
       </c>
+      <c r="CZ268" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="269" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>267</v>
       </c>
@@ -84887,8 +85701,11 @@
       <c r="CY269" t="s">
         <v>147</v>
       </c>
+      <c r="CZ269" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="270" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>262</v>
       </c>
@@ -85189,8 +86006,11 @@
       <c r="CY270">
         <v>0</v>
       </c>
+      <c r="CZ270" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="271" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>259</v>
       </c>
@@ -85491,8 +86311,11 @@
       <c r="CY271">
         <v>0</v>
       </c>
+      <c r="CZ271" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="272" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>255</v>
       </c>
@@ -85793,8 +86616,11 @@
       <c r="CY272" t="s">
         <v>51</v>
       </c>
+      <c r="CZ272" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="273" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>252</v>
       </c>
@@ -86095,8 +86921,11 @@
       <c r="CY273" t="s">
         <v>249</v>
       </c>
+      <c r="CZ273" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="274" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>248</v>
       </c>
@@ -86397,8 +87226,11 @@
       <c r="CY274">
         <v>0</v>
       </c>
+      <c r="CZ274" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="275" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>244</v>
       </c>
@@ -86699,8 +87531,11 @@
       <c r="CY275" t="s">
         <v>241</v>
       </c>
+      <c r="CZ275" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="276" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>240</v>
       </c>
@@ -87001,8 +87836,11 @@
       <c r="CY276" t="s">
         <v>237</v>
       </c>
+      <c r="CZ276" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="277" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>236</v>
       </c>
@@ -87303,8 +88141,11 @@
       <c r="CY277">
         <v>0</v>
       </c>
+      <c r="CZ277" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="278" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>233</v>
       </c>
@@ -87605,8 +88446,11 @@
       <c r="CY278" t="s">
         <v>51</v>
       </c>
+      <c r="CZ278" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="279" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>229</v>
       </c>
@@ -87907,8 +88751,11 @@
       <c r="CY279">
         <v>0</v>
       </c>
+      <c r="CZ279" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="280" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>224</v>
       </c>
@@ -88209,8 +89056,11 @@
       <c r="CY280" t="s">
         <v>171</v>
       </c>
+      <c r="CZ280" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="281" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>221</v>
       </c>
@@ -88511,8 +89361,11 @@
       <c r="CY281" t="s">
         <v>219</v>
       </c>
+      <c r="CZ281" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="282" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>218</v>
       </c>
@@ -88813,8 +89666,11 @@
       <c r="CY282" t="s">
         <v>214</v>
       </c>
+      <c r="CZ282" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="283" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>213</v>
       </c>
@@ -89115,8 +89971,11 @@
       <c r="CY283">
         <v>0</v>
       </c>
+      <c r="CZ283" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="284" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>207</v>
       </c>
@@ -89417,8 +90276,11 @@
       <c r="CY284" t="s">
         <v>203</v>
       </c>
+      <c r="CZ284" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="285" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>202</v>
       </c>
@@ -89719,8 +90581,11 @@
       <c r="CY285">
         <v>0</v>
       </c>
+      <c r="CZ285" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="286" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>199</v>
       </c>
@@ -90021,8 +90886,11 @@
       <c r="CY286">
         <v>0</v>
       </c>
+      <c r="CZ286" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="287" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>197</v>
       </c>
@@ -90323,8 +91191,11 @@
       <c r="CY287">
         <v>0</v>
       </c>
+      <c r="CZ287" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="288" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>194</v>
       </c>
@@ -90625,8 +91496,11 @@
       <c r="CY288" t="s">
         <v>190</v>
       </c>
+      <c r="CZ288" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="289" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>189</v>
       </c>
@@ -90927,8 +91801,11 @@
       <c r="CY289">
         <v>0</v>
       </c>
+      <c r="CZ289" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="290" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>186</v>
       </c>
@@ -91229,8 +92106,11 @@
       <c r="CY290" t="s">
         <v>133</v>
       </c>
+      <c r="CZ290" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="291" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>183</v>
       </c>
@@ -91531,8 +92411,11 @@
       <c r="CY291" t="s">
         <v>97</v>
       </c>
+      <c r="CZ291" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="292" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>181</v>
       </c>
@@ -91833,8 +92716,11 @@
       <c r="CY292" t="s">
         <v>178</v>
       </c>
+      <c r="CZ292" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="293" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>177</v>
       </c>
@@ -92135,8 +93021,11 @@
       <c r="CY293">
         <v>0</v>
       </c>
+      <c r="CZ293" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="294" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>174</v>
       </c>
@@ -92437,8 +93326,11 @@
       <c r="CY294" t="s">
         <v>171</v>
       </c>
+      <c r="CZ294" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="295" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>170</v>
       </c>
@@ -92739,8 +93631,11 @@
       <c r="CY295" t="s">
         <v>97</v>
       </c>
+      <c r="CZ295" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="296" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>167</v>
       </c>
@@ -93041,8 +93936,11 @@
       <c r="CY296">
         <v>0</v>
       </c>
+      <c r="CZ296" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="297" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>165</v>
       </c>
@@ -93343,8 +94241,11 @@
       <c r="CY297" t="s">
         <v>70</v>
       </c>
+      <c r="CZ297" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="298" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>160</v>
       </c>
@@ -93645,8 +94546,11 @@
       <c r="CY298" t="s">
         <v>154</v>
       </c>
+      <c r="CZ298" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="299" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>153</v>
       </c>
@@ -93947,8 +94851,11 @@
       <c r="CY299" t="s">
         <v>23</v>
       </c>
+      <c r="CZ299" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="300" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>150</v>
       </c>
@@ -94249,8 +95156,11 @@
       <c r="CY300" t="s">
         <v>147</v>
       </c>
+      <c r="CZ300" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="301" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>146</v>
       </c>
@@ -94551,8 +95461,11 @@
       <c r="CY301" t="s">
         <v>51</v>
       </c>
+      <c r="CZ301" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="302" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>142</v>
       </c>
@@ -94853,8 +95766,11 @@
       <c r="CY302" t="s">
         <v>137</v>
       </c>
+      <c r="CZ302" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="303" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>136</v>
       </c>
@@ -95155,8 +96071,11 @@
       <c r="CY303">
         <v>0</v>
       </c>
+      <c r="CZ303" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="304" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>132</v>
       </c>
@@ -95457,8 +96376,11 @@
       <c r="CY304" t="s">
         <v>51</v>
       </c>
+      <c r="CZ304" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="305" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>127</v>
       </c>
@@ -95759,8 +96681,11 @@
       <c r="CY305">
         <v>0</v>
       </c>
+      <c r="CZ305" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="306" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>123</v>
       </c>
@@ -96061,8 +96986,11 @@
       <c r="CY306" t="s">
         <v>22</v>
       </c>
+      <c r="CZ306" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="307" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>118</v>
       </c>
@@ -96363,8 +97291,11 @@
       <c r="CY307">
         <v>0</v>
       </c>
+      <c r="CZ307" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="308" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>114</v>
       </c>
@@ -96665,8 +97596,11 @@
       <c r="CY308">
         <v>0</v>
       </c>
+      <c r="CZ308" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="309" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>109</v>
       </c>
@@ -96967,8 +97901,11 @@
       <c r="CY309" t="s">
         <v>102</v>
       </c>
+      <c r="CZ309" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="310" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>101</v>
       </c>
@@ -97269,8 +98206,11 @@
       <c r="CY310">
         <v>0</v>
       </c>
+      <c r="CZ310" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="311" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>96</v>
       </c>
@@ -97571,8 +98511,11 @@
       <c r="CY311">
         <v>0</v>
       </c>
+      <c r="CZ311" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="312" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>94</v>
       </c>
@@ -97873,8 +98816,11 @@
       <c r="CY312">
         <v>0</v>
       </c>
+      <c r="CZ312" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="313" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>89</v>
       </c>
@@ -98175,8 +99121,11 @@
       <c r="CY313" t="s">
         <v>16</v>
       </c>
+      <c r="CZ313" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="314" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>86</v>
       </c>
@@ -98477,8 +99426,11 @@
       <c r="CY314">
         <v>0</v>
       </c>
+      <c r="CZ314" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="315" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>82</v>
       </c>
@@ -98779,8 +99731,11 @@
       <c r="CY315" t="s">
         <v>75</v>
       </c>
+      <c r="CZ315" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="316" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>74</v>
       </c>
@@ -99081,8 +100036,11 @@
       <c r="CY316">
         <v>0</v>
       </c>
+      <c r="CZ316" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="317" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>69</v>
       </c>
@@ -99383,8 +100341,11 @@
       <c r="CY317">
         <v>0</v>
       </c>
+      <c r="CZ317" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="318" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>64</v>
       </c>
@@ -99685,8 +100646,11 @@
       <c r="CY318">
         <v>0</v>
       </c>
+      <c r="CZ318" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="319" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>60</v>
       </c>
@@ -99987,8 +100951,11 @@
       <c r="CY319">
         <v>0</v>
       </c>
+      <c r="CZ319" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="320" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>55</v>
       </c>
@@ -100289,8 +101256,11 @@
       <c r="CY320" t="s">
         <v>50</v>
       </c>
+      <c r="CZ320" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="321" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>49</v>
       </c>
@@ -100591,8 +101561,11 @@
       <c r="CY321">
         <v>0</v>
       </c>
+      <c r="CZ321" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="322" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>45</v>
       </c>
@@ -100893,8 +101866,11 @@
       <c r="CY322">
         <v>0</v>
       </c>
+      <c r="CZ322" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="323" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>41</v>
       </c>
@@ -101195,8 +102171,11 @@
       <c r="CY323">
         <v>0</v>
       </c>
+      <c r="CZ323" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="324" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>36</v>
       </c>
@@ -101497,8 +102476,11 @@
       <c r="CY324" t="s">
         <v>29</v>
       </c>
+      <c r="CZ324" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="325" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>28</v>
       </c>
@@ -101799,8 +102781,11 @@
       <c r="CY325" t="s">
         <v>22</v>
       </c>
+      <c r="CZ325" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="326" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>21</v>
       </c>
@@ -102101,8 +103086,11 @@
       <c r="CY326">
         <v>0</v>
       </c>
+      <c r="CZ326" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="327" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>15</v>
       </c>
@@ -102403,8 +103391,11 @@
       <c r="CY327">
         <v>0</v>
       </c>
+      <c r="CZ327" t="s">
+        <v>1078</v>
+      </c>
     </row>
-    <row r="328" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:104" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>8</v>
       </c>
@@ -102704,10 +103695,14 @@
       </c>
       <c r="CY328" t="s">
         <v>0</v>
+      </c>
+      <c r="CZ328" t="s">
+        <v>1078</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>